<commit_message>
update répartition et WBS
</commit_message>
<xml_diff>
--- a/Soutenance finale/répartition.xlsx
+++ b/Soutenance finale/répartition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ponce\Desktop\IUT\Cours\ProjetTut\Projet-Tut-Documentation\Soutenance finale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD4F41F4-583E-4E7E-B9A9-7454CCD8D935}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADC53AD-35AA-4D3E-8658-7758153A8058}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{767348C1-9BFF-4DFE-A77D-EF6324554F75}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -679,7 +679,7 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
   </sheetData>

</xml_diff>